<commit_message>
Fixing inconsistency in data gathering
Now all the 3 inventories sum up to 1.
</commit_message>
<xml_diff>
--- a/Support data/Onshore wind.xlsx
+++ b/Support data/Onshore wind.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicog\Desktop\Nicolò\GitHub\GreenTechs\Support data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A7EC794-E6A3-473C-AB8F-B45D21B0FAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7A85D2-4556-49E9-8A80-95C28379A57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="19980" windowHeight="14190" autoFilterDateGrouping="0" xr2:uid="{00000000-0000-0000-0000-000000000000}"/>
+    <workbookView xWindow="30180" yWindow="1320" windowWidth="22980" windowHeight="12195" firstSheet="1" activeTab="3" autoFilterDateGrouping="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_Database levels" sheetId="4" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1850" uniqueCount="1555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1860" uniqueCount="1557">
   <si>
     <t>Scenario</t>
   </si>
@@ -4705,9 +4705,6 @@
     <t>Contingency</t>
   </si>
   <si>
-    <t>Consultancy, Land rent and Other financial costs</t>
-  </si>
-  <si>
     <t>Generator (DFIG)</t>
   </si>
   <si>
@@ -4727,6 +4724,15 @@
   </si>
   <si>
     <t>Value Added</t>
+  </si>
+  <si>
+    <t>Consultancy, Land rent and Other financial costs - engineering</t>
+  </si>
+  <si>
+    <t>Consultancy, Land rent and Other financial costs - construction</t>
+  </si>
+  <si>
+    <t>Consultancy, Land rent and Other financial costs - contingency</t>
   </si>
 </sst>
 </file>
@@ -4808,7 +4814,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4843,6 +4849,7 @@
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -5180,9 +5187,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5965D949-E255-4DFF-8B9B-61373D2891CE}">
   <dimension ref="A1:F1106"/>
   <sheetViews>
-    <sheetView showOutlineSymbols="0" defaultGridColor="0" showWhiteSpace="0" workbookViewId="0"/>
+    <sheetView showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="124.5546875" bestFit="1" customWidth="1"/>
@@ -11934,9 +11943,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59351A5-90BE-4DB0-876F-414402CEFD9C}">
   <dimension ref="A1:G1071"/>
   <sheetViews>
-    <sheetView showOutlineSymbols="0" defaultGridColor="0" showWhiteSpace="0" workbookViewId="0"/>
+    <sheetView showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.109375" customWidth="1"/>
     <col min="2" max="2" width="7.44140625" style="3" customWidth="1"/>
@@ -17376,9 +17385,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65393C0B-0C58-4933-9265-C2BD0E1A2DE5}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showOutlineSymbols="0" defaultGridColor="0" showWhiteSpace="0" workbookViewId="0"/>
+    <sheetView showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.88671875" bestFit="1" customWidth="1"/>
@@ -17440,7 +17451,7 @@
         <v>1532</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="C4" s="17">
         <f>19.6969696969697%*22.051965356429%</f>
@@ -17475,14 +17486,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEB86A8D-087F-40D1-B725-C3E6D23E7AC5}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showOutlineSymbols="0" defaultGridColor="0" showWhiteSpace="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.33203125" customWidth="1"/>
   </cols>
@@ -17566,7 +17579,7 @@
         <v>1532</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>1520</v>
@@ -17578,7 +17591,7 @@
         <v>1519</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -17591,8 +17604,8 @@
       <c r="C6" s="9" t="s">
         <v>1541</v>
       </c>
-      <c r="D6" s="15">
-        <v>3.0303030303030304E-2</v>
+      <c r="D6" s="20">
+        <v>3.7735849056603779E-2</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>4</v>
@@ -17609,8 +17622,8 @@
       <c r="C7" s="9" t="s">
         <v>1542</v>
       </c>
-      <c r="D7" s="15">
-        <v>0.23333333333333334</v>
+      <c r="D7" s="20">
+        <v>0.2905660377358491</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>4</v>
@@ -17627,8 +17640,8 @@
       <c r="C8" s="9" t="s">
         <v>1543</v>
       </c>
-      <c r="D8" s="15">
-        <v>0.12727272727272726</v>
+      <c r="D8" s="20">
+        <v>0.15849056603773584</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>4</v>
@@ -17645,8 +17658,8 @@
       <c r="C9" s="9" t="s">
         <v>1544</v>
       </c>
-      <c r="D9" s="15">
-        <v>0.41212121212121211</v>
+      <c r="D9" s="20">
+        <v>0.51320754716981132</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>4</v>
@@ -17699,9 +17712,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD44137B-885C-493B-A830-0D1C3B3D3991}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showOutlineSymbols="0" defaultGridColor="0" showWhiteSpace="0" workbookViewId="0"/>
+    <sheetView showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.5546875" bestFit="1" customWidth="1"/>
@@ -17847,7 +17862,7 @@
         <v>1539</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="D8" s="14">
         <v>0.3295432340532547</v>
@@ -18027,7 +18042,7 @@
         <v>1541</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>1547</v>
+        <v>1554</v>
       </c>
       <c r="D18" s="13">
         <v>1</v>
@@ -18045,7 +18060,7 @@
         <v>1545</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>1547</v>
+        <v>1555</v>
       </c>
       <c r="D19" s="10">
         <v>1</v>
@@ -18063,7 +18078,7 @@
         <v>1546</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>1547</v>
+        <v>1556</v>
       </c>
       <c r="D20" s="13">
         <v>1</v>
@@ -18080,11 +18095,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF714429-353E-4071-AE36-83A3774B3E41}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView showOutlineSymbols="0" defaultGridColor="0" showWhiteSpace="0" workbookViewId="0"/>
+    <sheetView showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68.33203125" bestFit="1" customWidth="1"/>
@@ -18292,7 +18309,7 @@
         <v>1532</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>28</v>
@@ -18502,7 +18519,7 @@
         <v>1532</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>1547</v>
+        <v>1554</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>27</v>
@@ -18515,6 +18532,48 @@
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="11" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="12">
+        <v>1</v>
+      </c>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>1556</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="12">
+        <v>1</v>
+      </c>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11" t="s">
         <v>1514</v>
       </c>
     </row>
@@ -18527,13 +18586,13 @@
           <x14:formula1>
             <xm:f>'_Database levels'!$B$2:$B$211</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D20</xm:sqref>
+          <xm:sqref>D2:D22</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{547D4329-6485-4BD8-81A3-E65A0C4E4CE4}">
           <x14:formula1>
             <xm:f>'_Database levels'!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C20</xm:sqref>
+          <xm:sqref>C2:C22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -18545,9 +18604,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E6C6C9B-2EDA-49F9-A91D-DFC94EE3C938}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showOutlineSymbols="0" defaultGridColor="0" showWhiteSpace="0" workbookViewId="0"/>
+    <sheetView showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.44140625" bestFit="1" customWidth="1"/>
@@ -18591,10 +18650,10 @@
         <v>3.7048340421245961E-2</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>1550</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>1551</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>1552</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
@@ -18613,10 +18672,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
@@ -18635,10 +18694,10 @@
         <v>0</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -18657,10 +18716,10 @@
         <v>6.5201917446804855E-3</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
@@ -18679,10 +18738,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
@@ -18701,10 +18760,10 @@
         <v>3.1358930747190712E-2</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -18723,10 +18782,10 @@
         <v>0.34722392325307005</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -18745,10 +18804,10 @@
         <v>0.26241843937473458</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -18767,10 +18826,10 @@
         <v>0.11659855418187548</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
@@ -18789,10 +18848,10 @@
         <v>0</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
@@ -18811,10 +18870,10 @@
         <v>0</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -18833,10 +18892,10 @@
         <v>0.19883162027720275</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -18862,9 +18921,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989882E4-2366-436B-8026-8EF8664D7F68}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showOutlineSymbols="0" defaultGridColor="0" showWhiteSpace="0" workbookViewId="0"/>
+    <sheetView showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
@@ -18883,7 +18942,7 @@
         <v>1532</v>
       </c>
       <c r="B2" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
     </row>
   </sheetData>
@@ -18895,9 +18954,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96ECECB5-F321-41F0-A4EC-C45486DF60C0}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showOutlineSymbols="0" defaultGridColor="0" showWhiteSpace="0" workbookViewId="0"/>
+    <sheetView showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="75.44140625" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>